<commit_message>
update program <in progress>
</commit_message>
<xml_diff>
--- a/Documents/Experiment-Design/experiment_design.xlsx
+++ b/Documents/Experiment-Design/experiment_design.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester3\Project-Module\Using-Image-Processing-for-Autonomous-Illumination-Sensor-Optimization\Documents\Experiment-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BFD6ED-6394-4D51-A938-2B2679EA71DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131EE0C-0429-4489-82C2-567F8F65F2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63C2CE48-B23F-428E-9F7D-E5F226C3B2C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{63C2CE48-B23F-428E-9F7D-E5F226C3B2C7}"/>
   </bookViews>
   <sheets>
     <sheet name="program" sheetId="2" r:id="rId1"/>
-    <sheet name="drawing" sheetId="1" r:id="rId2"/>
+    <sheet name="logics" sheetId="3" r:id="rId2"/>
+    <sheet name="drawing" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ultrasonic sensor</t>
   </si>
@@ -74,6 +75,27 @@
   </si>
   <si>
     <t>Person detect</t>
+  </si>
+  <si>
+    <t>Program Logics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective </t>
+  </si>
+  <si>
+    <t>To train a program for human-no human classification from top-view</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -2735,7 +2757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1D7E30-530D-4C7A-BA0E-137DB41EF95C}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -2782,6 +2804,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE7E135-2CC5-4344-8F2D-172EBE71202B}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA44C6-5B68-4D48-BABC-D7EE34EF441E}">
   <dimension ref="A1:L23"/>
   <sheetViews>

</xml_diff>

<commit_message>
program can now use roi features
</commit_message>
<xml_diff>
--- a/Documents/Experiment-Design/experiment_design.xlsx
+++ b/Documents/Experiment-Design/experiment_design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\Project-Module\Using-Image-Processing-for-Autonomous-Illumination-Sensor-Optimization\Documents\Experiment-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35413947-C971-42C0-AEBA-D04235401535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB8663-CCA1-4991-8DC6-D5DBF71EA9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63C2CE48-B23F-428E-9F7D-E5F226C3B2C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{63C2CE48-B23F-428E-9F7D-E5F226C3B2C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Program" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>ultrasonic sensor</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>STATE DIAGRAM</t>
+  </si>
+  <si>
+    <t>ROI logic creation</t>
   </si>
 </sst>
 </file>
@@ -21793,6 +21796,774 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7912067" cy="4323755"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34FD4DFC-1693-42F0-A155-A4E3BCAB791B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2424545" y="17196955"/>
+          <a:ext cx="7912067" cy="4323755"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>227157</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>319368</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>29136</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Oval 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{971FEF5E-E287-4C5E-B6B1-E3AA35085E94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3863975" y="17185749"/>
+          <a:ext cx="4941302" cy="4802842"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>425822</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>118782</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1908057" cy="1905000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Graphic 24" descr="Walk outline">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D939426C-5361-45A6-A428-79646A408E0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId28"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2850367" y="15029737"/>
+          <a:ext cx="1908057" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>146100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Arrow: Down 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41976DE7-7929-4B4E-9810-1CF0D39FEBC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19800000">
+          <a:off x="4343808" y="16614250"/>
+          <a:ext cx="1212272" cy="2443305"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> INCOMING</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>567017</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>84807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>567017</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>51612</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Arrow: Down 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B8E97C-79E6-4B84-9E96-BFF3BDC08285}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="12600000">
+          <a:off x="7234517" y="16519762"/>
+          <a:ext cx="1212273" cy="2443305"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> OUTGOING</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>582705</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1909076" cy="1905000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Graphic 29" descr="Walk outline">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE09088-4B5B-4D57-BFA3-C2F64556F51D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId28"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7856341" y="14910955"/>
+          <a:ext cx="1909076" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="TextBox 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD7BD792-87E3-4969-B699-565C0FAAEE4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5443003" y="18911455"/>
+          <a:ext cx="1818409" cy="605118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t>STAY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0"/>
+            <a:t> STILL</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>610027</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="TextBox 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B36577EC-1373-402B-97CB-9DE048FBBA11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1220055" y="29399073"/>
+          <a:ext cx="2440113" cy="611539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4472C4"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:shade val="50000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Click ROI button</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="TextBox 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF7E8CD-7526-465B-A073-F29D5E138D3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4270197" y="29399073"/>
+          <a:ext cx="3660168" cy="611539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4472C4"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:shade val="50000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pop up widow with image</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>610027</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="TextBox 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE40F73F-6B5C-4E73-88E3-F510973A65D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8540393" y="29399073"/>
+          <a:ext cx="3660168" cy="611539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4472C4"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:shade val="50000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>click on  points</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>610027</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>21403</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="TextBox 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B7816D-3E89-4B9A-BF62-4031ADAA02CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12810589" y="29399073"/>
+          <a:ext cx="5511657" cy="611539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4472C4"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:shade val="50000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>close window and return clicked positions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -24305,6 +25076,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="7" idx="7"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
@@ -24361,6 +25133,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="7" idx="0"/>
           <a:endCxn id="9" idx="0"/>
         </xdr:cNvCxnSpPr>
@@ -24497,6 +25270,590 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F9BA52-E6B1-4301-BFC3-C3164CD21432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10734675" y="6096000"/>
+          <a:ext cx="876300" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 283571"/>
+            <a:gd name="adj4" fmla="val -412831"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>58.52 cm</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7686675" cy="4323755"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7ABC863-0563-4C71-A623-A105E43A5C70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="6096000"/>
+          <a:ext cx="7686675" cy="4323755"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Oval 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2494DC0D-BBEC-48A7-B84C-4A7115817FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="8362950"/>
+          <a:ext cx="247649" cy="247649"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Callout: Line 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14BDDC4-954F-496D-9546-911CA7BADD51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10791825" y="7096125"/>
+          <a:ext cx="619125" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 253571"/>
+            <a:gd name="adj4" fmla="val -692179"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Center</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Oval 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95AF3138-BDD2-4AA1-AE6F-6E5534447B23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="6115050"/>
+          <a:ext cx="4914900" cy="4914900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Oval 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C305F888-49C8-426F-AA17-989A3B86F535}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4371975" y="6524625"/>
+          <a:ext cx="3971925" cy="3971925"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent5"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>97082</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>17217</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A87F7B4-A049-4A2E-BEB0-E60A432BE749}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6450257" y="7086600"/>
+          <a:ext cx="1322143" cy="1312617"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25047189-DCC9-478E-8F32-AA261CCC59BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="0"/>
+          <a:endCxn id="19" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6362700" y="6115050"/>
+          <a:ext cx="66675" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Callout: Line 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52EB110E-99EB-4944-8910-3543AF1E31FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10734675" y="5334000"/>
+          <a:ext cx="876300" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 288571"/>
+            <a:gd name="adj4" fmla="val -493266"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>94.8 cm</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Callout: Line 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48462815-31E3-44FC-A527-E583398114EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24860,7 +26217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1D7E30-530D-4C7A-BA0E-137DB41EF95C}">
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P99" sqref="P99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -24923,10 +26282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE7E135-2CC5-4344-8F2D-172EBE71202B}">
-  <dimension ref="A1:T134"/>
+  <dimension ref="A1:T149"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z138" sqref="Z138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25029,6 +26388,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25040,7 +26404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AA44C6-5B68-4D48-BABC-D7EE34EF441E}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:P49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -25123,8 +26489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7E79AB-3905-4B03-AA0A-D79715D3E696}">
   <dimension ref="A1:BC11"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BT52" sqref="BT52"/>
+    <sheetView showGridLines="0" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62:BC93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15"/>

</xml_diff>